<commit_message>
10/12/2019 data set update
</commit_message>
<xml_diff>
--- a/Project_2_Notes.v1.xlsx
+++ b/Project_2_Notes.v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asia8_000\Desktop\z.Temp\Rice_Data_Analytics_Boot_Camp\005 - Project.2\Higher_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879CE3F2-A23C-45A9-A7C9-894CDAD874FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E696A7F2-CA2D-49C2-9454-99137C88A7EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{540698A1-EA77-4181-9872-305E6C03902B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
   <si>
     <t>node is local version of JavaScript</t>
   </si>
@@ -339,12 +339,57 @@
   <si>
     <t>Data Set 4</t>
   </si>
+  <si>
+    <t>Project 2 and Project 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    D3 chart creation optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Bootstrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Plotly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   FLASK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   DB (postgres/mongodb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Herokku</t>
+  </si>
+  <si>
+    <t>The Annie E. Casey Foundation: Kids Count Data Center: Fourth grade reading achievement levels in the United States</t>
+  </si>
+  <si>
+    <t>https://factfinder.census.gov/faces/tableservices/jsf/pages/productview.xhtml?src=bkmk</t>
+  </si>
+  <si>
+    <t>American Fact Finder from Census Gov: Annual Survey of School System Finances: Per Pupil Amounts for Current Spending of Public Elementary-Secondary School Systems by State</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Richard | Gus</t>
+  </si>
+  <si>
+    <t>https://www.urban.org/policy-centers/cross-center-initiatives/state-and-local-finance-initiative/interactive-data-tools</t>
+  </si>
+  <si>
+    <t>Urban Institute: State and Local Finance Data Query System</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,8 +457,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,8 +486,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray"/>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -441,12 +504,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -459,35 +537,73 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -860,367 +976,788 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.44140625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="10"/>
-    <col min="5" max="5" width="9.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56" customWidth="1"/>
+    <col min="3" max="3" width="77.44140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="8"/>
+    <col min="5" max="5" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.6640625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="17" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="25" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="18">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="26"/>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="E6" s="27"/>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="C9" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="F9" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="17" t="s">
+      <c r="C10" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="32"/>
+    </row>
+    <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="27"/>
+      <c r="F12" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="17" t="s">
+    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="32"/>
+    </row>
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>73</v>
       </c>
+      <c r="E15" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="B18" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="33"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="33"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="33"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="33"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="33"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="33"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27" s="18">
         <v>3</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="23" t="s">
         <v>5</v>
       </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23" t="s">
         <v>25</v>
       </c>
+      <c r="C29" s="24"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="33"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23" t="s">
         <v>6</v>
       </c>
+      <c r="C30" s="24"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="33"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="33"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="33"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
+      <c r="A34" s="18">
         <v>4</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="26"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="33"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="22"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="33"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="33"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="33"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="11">
+      <c r="A39" s="18">
         <v>5</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="26"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="33"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="22"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="33"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="22"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="33"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="11">
+      <c r="A43" s="18">
         <v>6</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="26"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C44" s="17" t="s">
+      <c r="A44" s="22"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="22" t="s">
         <v>86</v>
       </c>
+      <c r="F44" s="33"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C45" s="17" t="s">
+      <c r="A45" s="22"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="22" t="s">
         <v>73</v>
       </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="33"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="22"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="33"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="22"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="33"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="22"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="33"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="22"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="33"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="22"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="33"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="11">
+      <c r="A51" s="18">
         <v>7</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="12"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="26"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C52" s="17" t="s">
+      <c r="A52" s="22"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="22" t="s">
         <v>73</v>
       </c>
+      <c r="E52" s="22"/>
+      <c r="F52" s="33"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C53" s="17" t="s">
+      <c r="A53" s="22"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="24" t="s">
         <v>12</v>
       </c>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="33"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C54" s="17" t="s">
+      <c r="A54" s="22"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="24" t="s">
         <v>13</v>
       </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="33"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C55" s="17" t="s">
+      <c r="A55" s="22"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="24" t="s">
         <v>14</v>
       </c>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="33"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C56" s="17" t="s">
+      <c r="A56" s="22"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="24" t="s">
         <v>15</v>
       </c>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="33"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C57" s="17" t="s">
+      <c r="A57" s="22"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="24" t="s">
         <v>17</v>
       </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="33"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C58" s="17" t="s">
+      <c r="A58" s="22"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="22" t="s">
         <v>65</v>
       </c>
+      <c r="E58" s="22"/>
+      <c r="F58" s="33"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="22"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="33"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="22"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="33"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="22"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="33"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="11">
+      <c r="A62" s="18">
         <v>8</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="12"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="26"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C63" s="17" t="s">
+      <c r="A63" s="22"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D63" s="22" t="s">
         <v>73</v>
       </c>
+      <c r="E63" s="22"/>
+      <c r="F63" s="33"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C64" s="17" t="s">
+      <c r="A64" s="22"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="24" t="s">
         <v>69</v>
       </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="33"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C65" s="17" t="s">
+      <c r="A65" s="22"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="24" t="s">
         <v>70</v>
       </c>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="33"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="22"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="33"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="11">
+      <c r="A67" s="18">
         <v>9</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="19"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="12"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="26"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="22"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="33"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="11">
+      <c r="A69" s="18">
         <v>10</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C69" s="19"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="12"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="26"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="22"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="33"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="22"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1228,6 +1765,8 @@
     <hyperlink ref="F8" r:id="rId2" location="detailed/2/2-52/false/871,573,36,867,38,18,16,14,13/1185,1186,1187,1188/11560" xr:uid="{3266094E-3565-4B31-8364-068063C22EFC}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{89E1990D-DC90-4C35-9AEC-62C7138BA1DC}"/>
     <hyperlink ref="F2" r:id="rId4" xr:uid="{601A7062-AC23-4F5C-A621-7DA9D40453F3}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{FBCBB904-66D7-490B-91E9-3D747656F26E}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{15C04F72-67CA-4319-BAAA-8925B113F66D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1235,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D17B82C-3E9F-4DF0-9B03-76BAF551C3A7}">
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,25 +2039,93 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
10/13/2019 completed python data cleaning and postgresql data push
</commit_message>
<xml_diff>
--- a/Project_2_Notes.v1.xlsx
+++ b/Project_2_Notes.v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asia8_000\Desktop\z.Temp\Rice_Data_Analytics_Boot_Camp\005 - Project.2\Higher_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D752EDE8-231E-41E7-9DCA-B1CDBA0C6BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEDD8A8-3B6E-4A14-96BD-4E78F9AFB316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{540698A1-EA77-4181-9872-305E6C03902B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="141">
   <si>
     <t>node is local version of JavaScript</t>
   </si>
@@ -388,15 +388,9 @@
     <t>Terminated</t>
   </si>
   <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
     <t>Set up tables</t>
   </si>
   <si>
-    <t>Import data</t>
-  </si>
-  <si>
     <t>Set up Team GitHub</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>column F &amp; C</t>
   </si>
   <si>
-    <t>Column C</t>
-  </si>
-  <si>
     <t>Use Enrollment and Total Expenditures</t>
   </si>
   <si>
@@ -494,6 +485,18 @@
   </si>
   <si>
     <t>10/14/2019 6:30pm</t>
+  </si>
+  <si>
+    <t>Data: PostgreSQL</t>
+  </si>
+  <si>
+    <t>Column C| Total Expenditure</t>
+  </si>
+  <si>
+    <t>Data: Python | PostgreSQL</t>
+  </si>
+  <si>
+    <t>Create code to import into Python and export to PostgreSQL</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,12 +634,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -666,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -787,9 +784,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1162,11 +1156,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1191,7 @@
         <v>85</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G1" s="40" t="s">
         <v>57</v>
@@ -1223,7 +1217,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
       <c r="B3" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>60</v>
@@ -1242,20 +1236,20 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1358,7 +1352,7 @@
         <v>87</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>100</v>
@@ -1377,7 +1371,7 @@
         <v>102</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>100</v>
@@ -1393,10 +1387,10 @@
     <row r="13" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="34"/>
       <c r="B13" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>100</v>
@@ -1406,16 +1400,16 @@
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>100</v>
@@ -1425,16 +1419,16 @@
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>100</v>
@@ -1444,7 +1438,7 @@
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1500,13 +1494,13 @@
         <v>99</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D19" s="36"/>
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
       <c r="G19" s="41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1534,7 +1528,7 @@
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1553,7 +1547,7 @@
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1568,11 +1562,11 @@
         <v>66</v>
       </c>
       <c r="E23" s="45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F23" s="45"/>
       <c r="G23" s="44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1581,7 +1575,7 @@
         <v>79</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>66</v>
@@ -1591,7 +1585,7 @@
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="32" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1600,7 +1594,7 @@
         <v>79</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>66</v>
@@ -1610,7 +1604,7 @@
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1619,17 +1613,17 @@
         <v>79</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>100</v>
       </c>
       <c r="E26" s="45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1638,7 +1632,7 @@
         <v>79</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D27" s="36" t="s">
         <v>100</v>
@@ -1648,7 +1642,7 @@
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1663,10 +1657,10 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="34"/>
       <c r="B29" s="35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D29" s="36" t="s">
         <v>84</v>
@@ -1693,17 +1687,17 @@
     <row r="31" spans="1:7" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="46"/>
       <c r="B31" s="47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D31" s="46" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="46"/>
       <c r="F31" s="48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G31" s="24"/>
     </row>
@@ -1713,14 +1707,14 @@
         <v>25</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D32" s="46" t="s">
         <v>73</v>
       </c>
       <c r="E32" s="46"/>
       <c r="F32" s="48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G32" s="24"/>
     </row>
@@ -1730,14 +1724,14 @@
         <v>6</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D33" s="46" t="s">
         <v>66</v>
       </c>
       <c r="E33" s="46"/>
       <c r="F33" s="48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G33" s="24"/>
     </row>
@@ -1980,11 +1974,11 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="22"/>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="32" t="s">
         <v>104</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>105</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>73</v>
@@ -1995,88 +1989,114 @@
     </row>
     <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="49" t="s">
+      <c r="B58" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
+      <c r="D58" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="F58" s="22"/>
       <c r="G58" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="22"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
+      <c r="B59" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="F59" s="22"/>
       <c r="G59" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="22"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
+      <c r="B60" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="F60" s="22"/>
       <c r="G60" s="32" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="22"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
+      <c r="B61" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="F61" s="22"/>
       <c r="G61" s="32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="22"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
+      <c r="B62" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="F62" s="22"/>
-      <c r="G62" s="29"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="22"/>
-      <c r="B63" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D63" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="29"/>
-    </row>
-    <row r="64" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="26"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="26"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="26"/>
-      <c r="G64" s="28"/>
+      <c r="G62" s="32"/>
+    </row>
+    <row r="63" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="26"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="28"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="22"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="29"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="22"/>
@@ -2089,7 +2109,9 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="22"/>
-      <c r="B66" s="24"/>
+      <c r="B66" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="C66" s="24"/>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
@@ -2099,7 +2121,7 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="22"/>
       <c r="B67" s="24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67" s="22"/>
@@ -2110,7 +2132,7 @@
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="22"/>
       <c r="B68" s="24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C68" s="24"/>
       <c r="D68" s="22"/>
@@ -2121,7 +2143,7 @@
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="22"/>
       <c r="B69" s="24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C69" s="24"/>
       <c r="D69" s="22"/>
@@ -2132,7 +2154,7 @@
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="22"/>
       <c r="B70" s="24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C70" s="24"/>
       <c r="D70" s="22"/>
@@ -2140,26 +2162,24 @@
       <c r="F70" s="22"/>
       <c r="G70" s="29"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="22"/>
       <c r="B71" s="24" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C71" s="24"/>
-      <c r="D71" s="22"/>
+      <c r="D71" s="22" t="s">
+        <v>65</v>
+      </c>
       <c r="E71" s="22"/>
       <c r="F71" s="22"/>
       <c r="G71" s="29"/>
     </row>
-    <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="22"/>
-      <c r="B72" s="24" t="s">
-        <v>74</v>
-      </c>
+      <c r="B72" s="23"/>
       <c r="C72" s="24"/>
-      <c r="D72" s="22" t="s">
-        <v>65</v>
-      </c>
+      <c r="D72" s="22"/>
       <c r="E72" s="22"/>
       <c r="F72" s="22"/>
       <c r="G72" s="29"/>
@@ -2183,36 +2203,38 @@
       <c r="G74" s="29"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="22"/>
-      <c r="B75" s="23"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="29"/>
+      <c r="A75" s="18">
+        <v>8</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="20"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="25"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="18">
-        <v>8</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C76" s="20"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="25"/>
+      <c r="A76" s="22"/>
+      <c r="B76" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" s="24"/>
+      <c r="D76" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="29"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="22"/>
       <c r="B77" s="24" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C77" s="24"/>
-      <c r="D77" s="22" t="s">
-        <v>73</v>
-      </c>
+      <c r="D77" s="22"/>
       <c r="E77" s="22"/>
       <c r="F77" s="22"/>
       <c r="G77" s="29"/>
@@ -2220,7 +2242,7 @@
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="22"/>
       <c r="B78" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C78" s="24"/>
       <c r="D78" s="22"/>
@@ -2230,9 +2252,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="22"/>
-      <c r="B79" s="24" t="s">
-        <v>70</v>
-      </c>
+      <c r="B79" s="23"/>
       <c r="C79" s="24"/>
       <c r="D79" s="22"/>
       <c r="E79" s="22"/>
@@ -2240,48 +2260,48 @@
       <c r="G79" s="29"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="22"/>
-      <c r="B80" s="23"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="29"/>
+      <c r="A80" s="18">
+        <v>9</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80" s="20"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="25"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="18">
-        <v>9</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C81" s="20"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="25"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="29"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="22"/>
-      <c r="B82" s="23"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="22"/>
-      <c r="G82" s="29"/>
+      <c r="A82" s="18">
+        <v>10</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C82" s="20"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="25"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="18">
-        <v>10</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C83" s="20"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="25"/>
+      <c r="A83" s="22"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="29"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="22"/>
@@ -2291,15 +2311,6 @@
       <c r="E84" s="22"/>
       <c r="F84" s="22"/>
       <c r="G84" s="29"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="22"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>